<commit_message>
adding TODOs after monday s meeting
Signed-off-by: Augusto Luis Ballardini <augusto.ballardini@uah.es>
</commit_message>
<xml_diff>
--- a/GAN/GAN.layer.calculator.xlsx
+++ b/GAN/GAN.layer.calculator.xlsx
@@ -99,12 +99,24 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF8000"/>
+        <bgColor rgb="FFFF6600"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF81D41A"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -144,7 +156,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -159,6 +171,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -215,9 +235,9 @@
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FF81D41A"/>
       <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF8000"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
@@ -239,13 +259,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="D2:J69"/>
+  <dimension ref="C2:J69"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B59" activeCellId="0" sqref="B59"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F44" activeCellId="0" sqref="F43:F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D2" s="1" t="s">
@@ -363,11 +383,13 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="4"/>
       <c r="D12" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="4"/>
       <c r="D13" s="3" t="s">
         <v>2</v>
       </c>
@@ -386,6 +408,7 @@
       <c r="I13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="4"/>
       <c r="D14" s="2" t="n">
         <v>1</v>
       </c>
@@ -407,6 +430,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="4"/>
       <c r="D15" s="2" t="n">
         <f aca="false">I14</f>
         <v>3</v>
@@ -429,6 +453,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="4"/>
       <c r="D16" s="2" t="n">
         <f aca="false">I15</f>
         <v>6</v>
@@ -451,6 +476,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="4"/>
       <c r="D17" s="2" t="n">
         <f aca="false">I16</f>
         <v>13</v>
@@ -473,6 +499,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="4"/>
       <c r="D18" s="2" t="n">
         <f aca="false">I17</f>
         <v>28</v>
@@ -495,6 +522,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="4"/>
       <c r="D19" s="2" t="n">
         <f aca="false">I18</f>
         <v>56</v>
@@ -517,6 +545,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="4"/>
       <c r="D20" s="2" t="n">
         <f aca="false">I19</f>
         <v>112</v>
@@ -538,13 +567,21 @@
         <v>224</v>
       </c>
     </row>
+    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="4"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C22" s="4"/>
+    </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C23" s="4"/>
       <c r="D23" s="2" t="s">
         <v>8</v>
       </c>
       <c r="J23" s="3"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="4"/>
       <c r="D24" s="3" t="s">
         <v>2</v>
       </c>
@@ -562,6 +599,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C25" s="4"/>
       <c r="D25" s="2" t="n">
         <v>224</v>
       </c>
@@ -583,6 +621,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C26" s="4"/>
       <c r="D26" s="2" t="n">
         <f aca="false">I25</f>
         <v>111</v>
@@ -605,6 +644,7 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C27" s="4"/>
       <c r="D27" s="2" t="n">
         <f aca="false">I26</f>
         <v>55</v>
@@ -627,6 +667,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C28" s="4"/>
       <c r="D28" s="2" t="n">
         <f aca="false">I27</f>
         <v>27</v>
@@ -649,6 +690,7 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C29" s="4"/>
       <c r="D29" s="2" t="n">
         <f aca="false">I28</f>
         <v>13</v>
@@ -671,6 +713,7 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C30" s="4"/>
       <c r="D30" s="2" t="n">
         <f aca="false">I29</f>
         <v>7</v>
@@ -693,6 +736,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="4"/>
       <c r="D31" s="2" t="n">
         <f aca="false">I30</f>
         <v>4</v>
@@ -715,6 +759,7 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C32" s="4"/>
       <c r="D32" s="2" t="n">
         <f aca="false">I31</f>
         <v>2</v>
@@ -750,11 +795,13 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C40" s="5"/>
       <c r="D40" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C41" s="5"/>
       <c r="D41" s="3" t="s">
         <v>2</v>
       </c>
@@ -773,6 +820,7 @@
       <c r="I41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C42" s="5"/>
       <c r="D42" s="2" t="n">
         <v>1</v>
       </c>
@@ -794,6 +842,7 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C43" s="5"/>
       <c r="D43" s="2" t="n">
         <f aca="false">I42</f>
         <v>3</v>
@@ -816,6 +865,7 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C44" s="5"/>
       <c r="D44" s="2" t="n">
         <f aca="false">I43</f>
         <v>6</v>
@@ -838,6 +888,7 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C45" s="5"/>
       <c r="D45" s="2" t="n">
         <f aca="false">I44</f>
         <v>13</v>
@@ -860,6 +911,7 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C46" s="5"/>
       <c r="D46" s="2" t="n">
         <f aca="false">I45</f>
         <v>27</v>
@@ -882,6 +934,7 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C47" s="5"/>
       <c r="D47" s="2" t="n">
         <f aca="false">I46</f>
         <v>55</v>
@@ -904,6 +957,7 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C48" s="5"/>
       <c r="D48" s="2" t="n">
         <f aca="false">I47</f>
         <v>111</v>
@@ -925,12 +979,20 @@
         <v>224</v>
       </c>
     </row>
+    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C49" s="5"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C50" s="5"/>
+    </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C51" s="5"/>
       <c r="D51" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C52" s="5"/>
       <c r="D52" s="3" t="s">
         <v>2</v>
       </c>
@@ -948,6 +1010,7 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C53" s="5"/>
       <c r="D53" s="2" t="n">
         <v>224</v>
       </c>
@@ -969,6 +1032,7 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C54" s="5"/>
       <c r="D54" s="2" t="n">
         <f aca="false">I53</f>
         <v>111</v>
@@ -991,6 +1055,7 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C55" s="5"/>
       <c r="D55" s="2" t="n">
         <f aca="false">I54</f>
         <v>55</v>
@@ -1013,6 +1078,7 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C56" s="5"/>
       <c r="D56" s="2" t="n">
         <f aca="false">I55</f>
         <v>27</v>
@@ -1035,6 +1101,7 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C57" s="5"/>
       <c r="D57" s="2" t="n">
         <f aca="false">I56</f>
         <v>13</v>
@@ -1057,6 +1124,7 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C58" s="5"/>
       <c r="D58" s="2" t="n">
         <f aca="false">I57</f>
         <v>6</v>
@@ -1079,6 +1147,7 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C59" s="5"/>
       <c r="D59" s="2" t="n">
         <f aca="false">I58</f>
         <v>3</v>

</xml_diff>

<commit_message>
Add UNet and Beefed-up generators
</commit_message>
<xml_diff>
--- a/GAN/GAN.layer.calculator.xlsx
+++ b/GAN/GAN.layer.calculator.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="22">
   <si>
     <t xml:space="preserve">https://pytorch.org/docs/stable/generated/torch.nn.ConvTranspose2d.html</t>
   </si>
@@ -52,13 +52,40 @@
     <t xml:space="preserve">CONV:</t>
   </si>
   <si>
-    <t xml:space="preserve">(W+2p-K-2) / S +1</t>
+    <t xml:space="preserve">[ (W+2p-K-2) / S ] +1</t>
   </si>
   <si>
     <t xml:space="preserve">TransposedConv: (W-1)S-2p +K</t>
   </si>
   <si>
     <t xml:space="preserve">Generator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generator beefed-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generator UNET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">upsample</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p3</t>
   </si>
 </sst>
 </file>
@@ -99,24 +126,12 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF8000"/>
-        <bgColor rgb="FFFF6600"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF81D41A"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -156,7 +171,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -171,14 +186,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -235,9 +242,9 @@
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF81D41A"/>
+      <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF8000"/>
+      <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
@@ -259,25 +266,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="C2:J69"/>
+  <dimension ref="D2:M94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F44" activeCellId="0" sqref="F43:F44"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K86" activeCellId="0" sqref="D86:K86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D4" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="3" t="s">
         <v>2</v>
       </c>
@@ -287,15 +294,18 @@
       <c r="F5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="3"/>
+      <c r="H5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="I5" s="3"/>
+      <c r="J5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="2" t="n">
         <v>1</v>
       </c>
@@ -305,20 +315,23 @@
       <c r="F6" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G6" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G6" s="2"/>
       <c r="H6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="2" t="n">
-        <f aca="false">(D6-1)*F6-2*H6+G6*(E6-1)+0+1</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2" t="n">
+        <f aca="false">(D6-1)*F6-2*J6+H6*(E6-1)+0+1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="2" t="n">
-        <f aca="false">I6</f>
+        <f aca="false">L6</f>
         <v>3</v>
       </c>
       <c r="E7" s="2" t="n">
@@ -327,20 +340,23 @@
       <c r="F7" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G7" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G7" s="2"/>
       <c r="H7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="2" t="n">
-        <f aca="false">(D7-1)*F7-2*H7+G7*(E7-1)+0+1</f>
+        <v>1</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2" t="n">
+        <f aca="false">(D7-1)*F7-2*J7+H7*(E7-1)+0+1</f>
         <v>6</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="2" t="n">
-        <f aca="false">I7</f>
+        <f aca="false">L7</f>
         <v>6</v>
       </c>
       <c r="E8" s="2" t="n">
@@ -349,20 +365,23 @@
       <c r="F8" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G8" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G8" s="2"/>
       <c r="H8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" s="2" t="n">
-        <f aca="false">(D8-1)*F8-2*H8+G8*(E8-1)+0+1</f>
+        <v>1</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2" t="n">
+        <f aca="false">(D8-1)*F8-2*J8+H8*(E8-1)+0+1</f>
         <v>13</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="2" t="n">
-        <f aca="false">I8</f>
+        <f aca="false">L8</f>
         <v>13</v>
       </c>
       <c r="E9" s="2" t="n">
@@ -371,25 +390,26 @@
       <c r="F9" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G9" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G9" s="2"/>
       <c r="H9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="2" t="n">
-        <f aca="false">(D9-1)*F9-2*H9+G9*(E9-1)+0+1</f>
+        <v>1</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2" t="n">
+        <f aca="false">(D9-1)*F9-2*J9+H9*(E9-1)+0+1</f>
         <v>28</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="4"/>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="4"/>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="3" t="s">
         <v>2</v>
       </c>
@@ -399,16 +419,18 @@
       <c r="F13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="3"/>
+      <c r="H13" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="I13" s="3"/>
+      <c r="J13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="4"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="2" t="n">
         <v>1</v>
       </c>
@@ -418,21 +440,23 @@
       <c r="F14" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G14" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G14" s="2"/>
       <c r="H14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" s="2" t="n">
-        <f aca="false">(D14-1)*F14-2*H14+G14*(E14-1)+0+1</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2" t="n">
+        <f aca="false">(D14-1)*F14-2*J14+H14*(E14-1)+0+1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D15" s="2" t="n">
-        <f aca="false">I14</f>
+        <f aca="false">L14</f>
         <v>3</v>
       </c>
       <c r="E15" s="2" t="n">
@@ -441,21 +465,23 @@
       <c r="F15" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G15" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G15" s="2"/>
       <c r="H15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I15" s="2" t="n">
-        <f aca="false">(D15-1)*F15-2*H15+G15*(E15-1)+0+1</f>
+        <v>1</v>
+      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2" t="n">
+        <f aca="false">(D15-1)*F15-2*J15+H15*(E15-1)+0+1</f>
         <v>6</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="4"/>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D16" s="2" t="n">
-        <f aca="false">I15</f>
+        <f aca="false">L15</f>
         <v>6</v>
       </c>
       <c r="E16" s="2" t="n">
@@ -464,21 +490,23 @@
       <c r="F16" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G16" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G16" s="2"/>
       <c r="H16" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I16" s="2" t="n">
-        <f aca="false">(D16-1)*F16-2*H16+G16*(E16-1)+0+1</f>
+        <v>1</v>
+      </c>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2" t="n">
+        <f aca="false">(D16-1)*F16-2*J16+H16*(E16-1)+0+1</f>
         <v>13</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="4"/>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D17" s="2" t="n">
-        <f aca="false">I16</f>
+        <f aca="false">L16</f>
         <v>13</v>
       </c>
       <c r="E17" s="2" t="n">
@@ -487,21 +515,23 @@
       <c r="F17" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G17" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G17" s="2"/>
       <c r="H17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I17" s="2" t="n">
-        <f aca="false">(D17-1)*F17-2*H17+G17*(E17-1)+0+1</f>
+        <v>1</v>
+      </c>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2" t="n">
+        <f aca="false">(D17-1)*F17-2*J17+H17*(E17-1)+0+1</f>
         <v>28</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="4"/>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D18" s="2" t="n">
-        <f aca="false">I17</f>
+        <f aca="false">L17</f>
         <v>28</v>
       </c>
       <c r="E18" s="2" t="n">
@@ -510,21 +540,23 @@
       <c r="F18" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G18" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G18" s="2"/>
       <c r="H18" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="I18" s="2" t="n">
-        <f aca="false">(D18-1)*F18-2*H18+G18*(E18-1)+0+1</f>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2" t="n">
+        <f aca="false">(D18-1)*F18-2*J18+H18*(E18-1)+0+1</f>
         <v>56</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="4"/>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D19" s="2" t="n">
-        <f aca="false">I18</f>
+        <f aca="false">L18</f>
         <v>56</v>
       </c>
       <c r="E19" s="2" t="n">
@@ -533,21 +565,23 @@
       <c r="F19" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G19" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G19" s="2"/>
       <c r="H19" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="I19" s="2" t="n">
-        <f aca="false">(D19-1)*F19-2*H19+G19*(E19-1)+0+1</f>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2" t="n">
+        <f aca="false">(D19-1)*F19-2*J19+H19*(E19-1)+0+1</f>
         <v>112</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="4"/>
       <c r="D20" s="2" t="n">
-        <f aca="false">I19</f>
+        <f aca="false">L19</f>
         <v>112</v>
       </c>
       <c r="E20" s="2" t="n">
@@ -556,32 +590,27 @@
       <c r="F20" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G20" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G20" s="2"/>
       <c r="H20" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="I20" s="2" t="n">
-        <f aca="false">(D20-1)*F20-2*H20+G20*(E20-1)+0+1</f>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2" t="n">
+        <f aca="false">(D20-1)*F20-2*J20+H20*(E20-1)+0+1</f>
         <v>224</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="4"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="4"/>
-    </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="4"/>
       <c r="D23" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J23" s="3"/>
+      <c r="M23" s="3"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="4"/>
       <c r="D24" s="3" t="s">
         <v>2</v>
       </c>
@@ -591,15 +620,17 @@
       <c r="F24" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="G24" s="3"/>
+      <c r="H24" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="I24" s="3"/>
+      <c r="J24" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="K24" s="3"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="4"/>
       <c r="D25" s="2" t="n">
         <v>224</v>
       </c>
@@ -609,21 +640,23 @@
       <c r="F25" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G25" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G25" s="2"/>
       <c r="H25" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I25" s="2" t="n">
-        <f aca="false">((D25+2*H25-G25*(E25-1)-1)/F25)+1</f>
+        <v>1</v>
+      </c>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2" t="n">
+        <f aca="false">((D25+2*J25-H25*(E25-1)-1)/F25)+1</f>
         <v>111</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="4"/>
       <c r="D26" s="2" t="n">
-        <f aca="false">I25</f>
+        <f aca="false">L25</f>
         <v>111</v>
       </c>
       <c r="E26" s="2" t="n">
@@ -632,21 +665,23 @@
       <c r="F26" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G26" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G26" s="2"/>
       <c r="H26" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I26" s="2" t="n">
-        <f aca="false">((D26+2*H26-G26*(E26-1)-1)/F26)+1</f>
+        <v>1</v>
+      </c>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2" t="n">
+        <f aca="false">((D26+2*J26-H26*(E26-1)-1)/F26)+1</f>
         <v>55</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="4"/>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D27" s="2" t="n">
-        <f aca="false">I26</f>
+        <f aca="false">L26</f>
         <v>55</v>
       </c>
       <c r="E27" s="2" t="n">
@@ -655,21 +690,23 @@
       <c r="F27" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G27" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G27" s="2"/>
       <c r="H27" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I27" s="2" t="n">
-        <f aca="false">((D27+2*H27-G27*(E27-1)-1)/F27)+1</f>
+        <v>1</v>
+      </c>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2" t="n">
+        <f aca="false">((D27+2*J27-H27*(E27-1)-1)/F27)+1</f>
         <v>27</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="4"/>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D28" s="2" t="n">
-        <f aca="false">I27</f>
+        <f aca="false">L27</f>
         <v>27</v>
       </c>
       <c r="E28" s="2" t="n">
@@ -678,21 +715,23 @@
       <c r="F28" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G28" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G28" s="2"/>
       <c r="H28" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I28" s="2" t="n">
-        <f aca="false">((D28+2*H28-G28*(E28-1)-1)/F28)+1</f>
+        <v>1</v>
+      </c>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2" t="n">
+        <f aca="false">((D28+2*J28-H28*(E28-1)-1)/F28)+1</f>
         <v>13</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="4"/>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D29" s="2" t="n">
-        <f aca="false">I28</f>
+        <f aca="false">L28</f>
         <v>13</v>
       </c>
       <c r="E29" s="2" t="n">
@@ -701,21 +740,23 @@
       <c r="F29" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G29" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G29" s="2"/>
       <c r="H29" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="I29" s="2" t="n">
-        <f aca="false">((D29+2*H29-G29*(E29-1)-1)/F29)+1</f>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2" t="n">
+        <f aca="false">((D29+2*J29-H29*(E29-1)-1)/F29)+1</f>
         <v>7</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="4"/>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D30" s="2" t="n">
-        <f aca="false">I29</f>
+        <f aca="false">L29</f>
         <v>7</v>
       </c>
       <c r="E30" s="2" t="n">
@@ -724,21 +765,23 @@
       <c r="F30" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G30" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G30" s="2"/>
       <c r="H30" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="I30" s="2" t="n">
-        <f aca="false">((D30+2*H30-G30*(E30-1)-1)/F30)+1</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="4"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2" t="n">
+        <f aca="false">((D30+2*J30-H30*(E30-1)-1)/F30)+1</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D31" s="2" t="n">
-        <f aca="false">I30</f>
+        <f aca="false">L30</f>
         <v>4</v>
       </c>
       <c r="E31" s="2" t="n">
@@ -747,21 +790,23 @@
       <c r="F31" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G31" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G31" s="2"/>
       <c r="H31" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="I31" s="2" t="n">
-        <f aca="false">((D31+2*H31-G31*(E31-1)-1)/F31)+1</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="4"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2" t="n">
+        <f aca="false">((D31+2*J31-H31*(E31-1)-1)/F31)+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D32" s="2" t="n">
-        <f aca="false">I31</f>
+        <f aca="false">L31</f>
         <v>2</v>
       </c>
       <c r="E32" s="2" t="n">
@@ -770,38 +815,42 @@
       <c r="F32" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G32" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G32" s="2"/>
       <c r="H32" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="I32" s="2" t="n">
-        <f aca="false">((D32+2*H32-G32*(E32-1)-1)/F32)+1</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I32" s="2"/>
+      <c r="J32" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2" t="n">
+        <f aca="false">((D32+2*J32-H32*(E32-1)-1)/F32)+1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F36" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="G36" s="2"/>
+      <c r="H36" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I36" s="2"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F37" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C40" s="5"/>
+      <c r="G37" s="2"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D40" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C41" s="5"/>
       <c r="D41" s="3" t="s">
         <v>2</v>
       </c>
@@ -811,16 +860,18 @@
       <c r="F41" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G41" s="3" t="s">
+      <c r="G41" s="3"/>
+      <c r="H41" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H41" s="3" t="s">
+      <c r="I41" s="3"/>
+      <c r="J41" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I41" s="3"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C42" s="5"/>
       <c r="D42" s="2" t="n">
         <v>1</v>
       </c>
@@ -830,21 +881,23 @@
       <c r="F42" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G42" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G42" s="2"/>
       <c r="H42" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I42" s="2" t="n">
-        <f aca="false">(D42-1)*F42-2*H42+G42*(E42-1)+0+1</f>
+        <v>1</v>
+      </c>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2" t="n">
+        <f aca="false">(D42-1)*F42-2*J42+H42*(E42-1)+0+1</f>
         <v>3</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C43" s="5"/>
       <c r="D43" s="2" t="n">
-        <f aca="false">I42</f>
+        <f aca="false">L42</f>
         <v>3</v>
       </c>
       <c r="E43" s="2" t="n">
@@ -853,21 +906,23 @@
       <c r="F43" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G43" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G43" s="2"/>
       <c r="H43" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I43" s="2" t="n">
-        <f aca="false">(D43-1)*F43-2*H43+G43*(E43-1)+0+1</f>
+        <v>1</v>
+      </c>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2" t="n">
+        <f aca="false">(D43-1)*F43-2*J43+H43*(E43-1)+0+1</f>
         <v>6</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C44" s="5"/>
       <c r="D44" s="2" t="n">
-        <f aca="false">I43</f>
+        <f aca="false">L43</f>
         <v>6</v>
       </c>
       <c r="E44" s="2" t="n">
@@ -876,21 +931,23 @@
       <c r="F44" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G44" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G44" s="2"/>
       <c r="H44" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I44" s="2" t="n">
-        <f aca="false">(D44-1)*F44-2*H44+G44*(E44-1)+0+1</f>
+        <v>1</v>
+      </c>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2" t="n">
+        <f aca="false">(D44-1)*F44-2*J44+H44*(E44-1)+0+1</f>
         <v>13</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C45" s="5"/>
       <c r="D45" s="2" t="n">
-        <f aca="false">I44</f>
+        <f aca="false">L44</f>
         <v>13</v>
       </c>
       <c r="E45" s="2" t="n">
@@ -899,21 +956,23 @@
       <c r="F45" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G45" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G45" s="2"/>
       <c r="H45" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I45" s="2" t="n">
-        <f aca="false">(D45-1)*F45-2*H45+G45*(E45-1)+0+1</f>
+        <v>1</v>
+      </c>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2" t="n">
+        <f aca="false">(D45-1)*F45-2*J45+H45*(E45-1)+0+1</f>
         <v>27</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C46" s="5"/>
       <c r="D46" s="2" t="n">
-        <f aca="false">I45</f>
+        <f aca="false">L45</f>
         <v>27</v>
       </c>
       <c r="E46" s="2" t="n">
@@ -922,21 +981,23 @@
       <c r="F46" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G46" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G46" s="2"/>
       <c r="H46" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I46" s="2" t="n">
-        <f aca="false">(D46-1)*F46-2*H46+G46*(E46-1)+0+1</f>
+        <v>1</v>
+      </c>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2" t="n">
+        <f aca="false">(D46-1)*F46-2*J46+H46*(E46-1)+0+1</f>
         <v>55</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C47" s="5"/>
       <c r="D47" s="2" t="n">
-        <f aca="false">I46</f>
+        <f aca="false">L46</f>
         <v>55</v>
       </c>
       <c r="E47" s="2" t="n">
@@ -945,21 +1006,23 @@
       <c r="F47" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G47" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G47" s="2"/>
       <c r="H47" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I47" s="2" t="n">
-        <f aca="false">(D47-1)*F47-2*H47+G47*(E47-1)+0+1</f>
+        <v>1</v>
+      </c>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2" t="n">
+        <f aca="false">(D47-1)*F47-2*J47+H47*(E47-1)+0+1</f>
         <v>111</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C48" s="5"/>
       <c r="D48" s="2" t="n">
-        <f aca="false">I47</f>
+        <f aca="false">L47</f>
         <v>111</v>
       </c>
       <c r="E48" s="2" t="n">
@@ -968,31 +1031,26 @@
       <c r="F48" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G48" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G48" s="2"/>
       <c r="H48" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I48" s="2" t="n">
-        <f aca="false">(D48-1)*F48-2*H48+G48*(E48-1)+0+1</f>
+        <v>1</v>
+      </c>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2" t="n">
+        <f aca="false">(D48-1)*F48-2*J48+H48*(E48-1)+0+1</f>
         <v>224</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C49" s="5"/>
-    </row>
-    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C50" s="5"/>
-    </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C51" s="5"/>
       <c r="D51" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C52" s="5"/>
       <c r="D52" s="3" t="s">
         <v>2</v>
       </c>
@@ -1002,15 +1060,17 @@
       <c r="F52" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G52" s="3" t="s">
+      <c r="G52" s="3"/>
+      <c r="H52" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H52" s="3" t="s">
+      <c r="I52" s="3"/>
+      <c r="J52" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="K52" s="3"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C53" s="5"/>
       <c r="D53" s="2" t="n">
         <v>224</v>
       </c>
@@ -1020,21 +1080,23 @@
       <c r="F53" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G53" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G53" s="2"/>
       <c r="H53" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I53" s="2" t="n">
-        <f aca="false">((D53+2*H53-G53*(E53-1)-1)/F53)+1</f>
+        <v>1</v>
+      </c>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K53" s="2"/>
+      <c r="L53" s="2" t="n">
+        <f aca="false">((D53+2*J53-H53*(E53-1)-1)/F53)+1</f>
         <v>111</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C54" s="5"/>
       <c r="D54" s="2" t="n">
-        <f aca="false">I53</f>
+        <f aca="false">L53</f>
         <v>111</v>
       </c>
       <c r="E54" s="2" t="n">
@@ -1043,21 +1105,23 @@
       <c r="F54" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G54" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G54" s="2"/>
       <c r="H54" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I54" s="2" t="n">
-        <f aca="false">((D54+2*H54-G54*(E54-1)-1)/F54)+1</f>
+        <v>1</v>
+      </c>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K54" s="2"/>
+      <c r="L54" s="2" t="n">
+        <f aca="false">((D54+2*J54-H54*(E54-1)-1)/F54)+1</f>
         <v>55</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C55" s="5"/>
       <c r="D55" s="2" t="n">
-        <f aca="false">I54</f>
+        <f aca="false">L54</f>
         <v>55</v>
       </c>
       <c r="E55" s="2" t="n">
@@ -1066,21 +1130,23 @@
       <c r="F55" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G55" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G55" s="2"/>
       <c r="H55" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I55" s="2" t="n">
-        <f aca="false">((D55+2*H55-G55*(E55-1)-1)/F55)+1</f>
+        <v>1</v>
+      </c>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K55" s="2"/>
+      <c r="L55" s="2" t="n">
+        <f aca="false">((D55+2*J55-H55*(E55-1)-1)/F55)+1</f>
         <v>27</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C56" s="5"/>
       <c r="D56" s="2" t="n">
-        <f aca="false">I55</f>
+        <f aca="false">L55</f>
         <v>27</v>
       </c>
       <c r="E56" s="2" t="n">
@@ -1089,21 +1155,23 @@
       <c r="F56" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G56" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G56" s="2"/>
       <c r="H56" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I56" s="2" t="n">
-        <f aca="false">((D56+2*H56-G56*(E56-1)-1)/F56)+1</f>
+        <v>1</v>
+      </c>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K56" s="2"/>
+      <c r="L56" s="2" t="n">
+        <f aca="false">((D56+2*J56-H56*(E56-1)-1)/F56)+1</f>
         <v>13</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C57" s="5"/>
       <c r="D57" s="2" t="n">
-        <f aca="false">I56</f>
+        <f aca="false">L56</f>
         <v>13</v>
       </c>
       <c r="E57" s="2" t="n">
@@ -1112,21 +1180,23 @@
       <c r="F57" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G57" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G57" s="2"/>
       <c r="H57" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I57" s="2" t="n">
-        <f aca="false">((D57+2*H57-G57*(E57-1)-1)/F57)+1</f>
+        <v>1</v>
+      </c>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K57" s="2"/>
+      <c r="L57" s="2" t="n">
+        <f aca="false">((D57+2*J57-H57*(E57-1)-1)/F57)+1</f>
         <v>6</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C58" s="5"/>
       <c r="D58" s="2" t="n">
-        <f aca="false">I57</f>
+        <f aca="false">L57</f>
         <v>6</v>
       </c>
       <c r="E58" s="2" t="n">
@@ -1135,21 +1205,23 @@
       <c r="F58" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G58" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G58" s="2"/>
       <c r="H58" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I58" s="2" t="n">
-        <f aca="false">((D58+2*H58-G58*(E58-1)-1)/F58)+1</f>
+        <v>1</v>
+      </c>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K58" s="2"/>
+      <c r="L58" s="2" t="n">
+        <f aca="false">((D58+2*J58-H58*(E58-1)-1)/F58)+1</f>
         <v>3</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C59" s="5"/>
       <c r="D59" s="2" t="n">
-        <f aca="false">I58</f>
+        <f aca="false">L58</f>
         <v>3</v>
       </c>
       <c r="E59" s="2" t="n">
@@ -1158,14 +1230,17 @@
       <c r="F59" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G59" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G59" s="2"/>
       <c r="H59" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I59" s="2" t="n">
-        <f aca="false">((D59+2*H59-G59*(E59-1)-1)/F59)+1</f>
+        <v>1</v>
+      </c>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K59" s="2"/>
+      <c r="L59" s="2" t="n">
+        <f aca="false">((D59+2*J59-H59*(E59-1)-1)/F59)+1</f>
         <v>1</v>
       </c>
     </row>
@@ -1175,63 +1250,611 @@
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="I60" s="2"/>
+      <c r="J60" s="2"/>
+      <c r="K60" s="2"/>
+    </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D63" s="2"/>
+      <c r="D63" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
+      <c r="J63" s="2"/>
+      <c r="K63" s="2"/>
+      <c r="L63" s="2"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D64" s="2"/>
-      <c r="E64" s="2"/>
-      <c r="F64" s="2"/>
-      <c r="G64" s="2"/>
-      <c r="H64" s="2"/>
-      <c r="I64" s="2"/>
+      <c r="D64" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G64" s="3"/>
+      <c r="H64" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I64" s="3"/>
+      <c r="J64" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K64" s="3"/>
+      <c r="L64" s="3"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D65" s="2"/>
-      <c r="E65" s="2"/>
-      <c r="F65" s="2"/>
+      <c r="D65" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E65" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="F65" s="2" t="n">
+        <v>2</v>
+      </c>
       <c r="G65" s="2"/>
-      <c r="H65" s="2"/>
+      <c r="H65" s="2" t="n">
+        <v>1</v>
+      </c>
       <c r="I65" s="2"/>
+      <c r="J65" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K65" s="2"/>
+      <c r="L65" s="2" t="n">
+        <f aca="false">(D65-1)*F65-2*J65+H65*(E65-1)+0+1</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D66" s="2"/>
-      <c r="E66" s="2"/>
-      <c r="F66" s="2"/>
+      <c r="D66" s="2" t="n">
+        <f aca="false">L65</f>
+        <v>3</v>
+      </c>
+      <c r="E66" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="F66" s="2" t="n">
+        <v>2</v>
+      </c>
       <c r="G66" s="2"/>
-      <c r="H66" s="2"/>
+      <c r="H66" s="2" t="n">
+        <v>1</v>
+      </c>
       <c r="I66" s="2"/>
+      <c r="J66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K66" s="2"/>
+      <c r="L66" s="2" t="n">
+        <f aca="false">(D66-1)*F66-2*J66+H66*(E66-1)+0+1</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D67" s="2"/>
-      <c r="E67" s="2"/>
-      <c r="F67" s="2"/>
+      <c r="D67" s="2" t="n">
+        <f aca="false">L66</f>
+        <v>7</v>
+      </c>
+      <c r="E67" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="F67" s="2" t="n">
+        <v>2</v>
+      </c>
       <c r="G67" s="2"/>
-      <c r="H67" s="2"/>
+      <c r="H67" s="2" t="n">
+        <v>1</v>
+      </c>
       <c r="I67" s="2"/>
+      <c r="J67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K67" s="2"/>
+      <c r="L67" s="2" t="n">
+        <f aca="false">(D67-1)*F67-2*J67+H67*(E67-1)+0+1</f>
+        <v>15</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D68" s="2"/>
-      <c r="E68" s="2"/>
-      <c r="F68" s="2"/>
+      <c r="D68" s="2" t="n">
+        <f aca="false">L67</f>
+        <v>15</v>
+      </c>
+      <c r="E68" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="F68" s="2" t="n">
+        <v>1</v>
+      </c>
       <c r="G68" s="2"/>
-      <c r="H68" s="2"/>
+      <c r="H68" s="2" t="n">
+        <v>1</v>
+      </c>
       <c r="I68" s="2"/>
+      <c r="J68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K68" s="2"/>
+      <c r="L68" s="2" t="n">
+        <f aca="false">(D68-1)*F68-2*J68+H68*(E68-1)+0+1</f>
+        <v>17</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D69" s="2"/>
-      <c r="E69" s="2"/>
-      <c r="F69" s="2"/>
+      <c r="D69" s="2" t="n">
+        <f aca="false">L68</f>
+        <v>17</v>
+      </c>
+      <c r="E69" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="F69" s="2" t="n">
+        <v>1</v>
+      </c>
       <c r="G69" s="2"/>
-      <c r="H69" s="2"/>
+      <c r="H69" s="2" t="n">
+        <v>1</v>
+      </c>
       <c r="I69" s="2"/>
+      <c r="J69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K69" s="2"/>
+      <c r="L69" s="2" t="n">
+        <f aca="false">(D69-1)*F69-2*J69+H69*(E69-1)+0+1</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D70" s="2" t="n">
+        <f aca="false">L69</f>
+        <v>20</v>
+      </c>
+      <c r="E70" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="F70" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G70" s="2"/>
+      <c r="H70" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I70" s="2"/>
+      <c r="J70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K70" s="2"/>
+      <c r="L70" s="2" t="n">
+        <f aca="false">(D70-1)*F70-2*J70+H70*(E70-1)+0+1</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D71" s="2" t="n">
+        <f aca="false">L70</f>
+        <v>22</v>
+      </c>
+      <c r="E71" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="F71" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G71" s="2"/>
+      <c r="H71" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I71" s="2"/>
+      <c r="J71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K71" s="2"/>
+      <c r="L71" s="2" t="n">
+        <f aca="false">(D71-1)*F71-2*J71+H71*(E71-1)+0+1</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D72" s="2" t="n">
+        <f aca="false">L71</f>
+        <v>24</v>
+      </c>
+      <c r="E72" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="F72" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G72" s="2"/>
+      <c r="H72" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I72" s="2"/>
+      <c r="J72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K72" s="2"/>
+      <c r="L72" s="2" t="n">
+        <f aca="false">(D72-1)*F72-2*J72+H72*(E72-1)+0+1</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D73" s="2" t="n">
+        <f aca="false">L72</f>
+        <v>27</v>
+      </c>
+      <c r="E73" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="F73" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G73" s="2"/>
+      <c r="H73" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I73" s="2"/>
+      <c r="J73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K73" s="2"/>
+      <c r="L73" s="2" t="n">
+        <f aca="false">(D73-1)*F73-2*J73+H73*(E73-1)+0+1</f>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D74" s="2" t="n">
+        <f aca="false">L73</f>
+        <v>56</v>
+      </c>
+      <c r="E74" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="F74" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G74" s="2"/>
+      <c r="H74" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I74" s="2"/>
+      <c r="J74" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K74" s="2"/>
+      <c r="L74" s="2" t="n">
+        <f aca="false">(D74-1)*F74-2*J74+H74*(E74-1)+0+1</f>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D75" s="2" t="n">
+        <f aca="false">L74</f>
+        <v>111</v>
+      </c>
+      <c r="E75" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="F75" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G75" s="2"/>
+      <c r="H75" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I75" s="2"/>
+      <c r="J75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K75" s="2"/>
+      <c r="L75" s="2" t="n">
+        <f aca="false">(D75-1)*F75-2*J75+H75*(E75-1)+0+1</f>
+        <v>224</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D82" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+      <c r="G82" s="2"/>
+      <c r="H82" s="2"/>
+      <c r="I82" s="2"/>
+      <c r="J82" s="2"/>
+      <c r="K82" s="2"/>
+      <c r="L82" s="2"/>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D83" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G83" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H83" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I83" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J83" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K83" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L83" s="3"/>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D84" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E84" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F84" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G84" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H84" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I84" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J84" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K84" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L84" s="2" t="n">
+        <f aca="false">(D84*E84)-F84+2*G84-H84+2*I84-J84+2*K84</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D85" s="2" t="n">
+        <f aca="false">L84</f>
+        <v>5</v>
+      </c>
+      <c r="E85" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F85" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G85" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H85" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I85" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J85" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K85" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L85" s="2" t="n">
+        <f aca="false">(D85*E85)-F85+2*G85-H85+2*I85-J85+2*K85</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D86" s="2" t="n">
+        <f aca="false">L85</f>
+        <v>13</v>
+      </c>
+      <c r="E86" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F86" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H86" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="I86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J86" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="K86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L86" s="2" t="n">
+        <f aca="false">(D86*E86)-F86+2*G86-H86+2*I86-J86+2*K86</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D87" s="2" t="n">
+        <f aca="false">L86</f>
+        <v>18</v>
+      </c>
+      <c r="E87" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F87" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G87" s="2"/>
+      <c r="H87" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="I87" s="2"/>
+      <c r="J87" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="K87" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L87" s="2" t="n">
+        <f aca="false">(D87*E87)-F87+2*G87-H87+2*I87-J87+2*K87</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D88" s="2" t="n">
+        <f aca="false">L87</f>
+        <v>30</v>
+      </c>
+      <c r="E88" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F88" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G88" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H88" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="I88" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J88" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="K88" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L88" s="2" t="n">
+        <f aca="false">(D88*E88)-F88+2*G88-H88+2*I88-J88+2*K88</f>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D89" s="2" t="n">
+        <f aca="false">L88</f>
+        <v>58</v>
+      </c>
+      <c r="E89" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F89" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G89" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H89" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="I89" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J89" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="K89" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L89" s="2" t="n">
+        <f aca="false">(D89*E89)-F89+2*G89-H89+2*I89-J89+2*K89</f>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D90" s="2" t="n">
+        <f aca="false">L89</f>
+        <v>114</v>
+      </c>
+      <c r="E90" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F90" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G90" s="2"/>
+      <c r="H90" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="I90" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J90" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="K90" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L90" s="2" t="n">
+        <f aca="false">(D90*E90)-F90+2*G90-H90+2*I90-J90+2*K90</f>
+        <v>224</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D91" s="2"/>
+      <c r="E91" s="2"/>
+      <c r="F91" s="2"/>
+      <c r="G91" s="2"/>
+      <c r="H91" s="2"/>
+      <c r="I91" s="2"/>
+      <c r="J91" s="2"/>
+      <c r="K91" s="2"/>
+      <c r="L91" s="2"/>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D92" s="2"/>
+      <c r="E92" s="2"/>
+      <c r="F92" s="2"/>
+      <c r="G92" s="2"/>
+      <c r="H92" s="2"/>
+      <c r="I92" s="2"/>
+      <c r="J92" s="2"/>
+      <c r="K92" s="2"/>
+      <c r="L92" s="2"/>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D93" s="2"/>
+      <c r="E93" s="2"/>
+      <c r="F93" s="2"/>
+      <c r="G93" s="2"/>
+      <c r="H93" s="2"/>
+      <c r="I93" s="2"/>
+      <c r="J93" s="2"/>
+      <c r="K93" s="2"/>
+      <c r="L93" s="2"/>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D94" s="2"/>
+      <c r="E94" s="2"/>
+      <c r="F94" s="2"/>
+      <c r="G94" s="2"/>
+      <c r="H94" s="2"/>
+      <c r="I94" s="2"/>
+      <c r="J94" s="2"/>
+      <c r="K94" s="2"/>
+      <c r="L94" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Add DCGAN layers and new config
</commit_message>
<xml_diff>
--- a/GAN/GAN.layer.calculator.xlsx
+++ b/GAN/GAN.layer.calculator.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="26">
   <si>
     <t xml:space="preserve">https://pytorch.org/docs/stable/generated/torch.nn.ConvTranspose2d.html</t>
   </si>
@@ -62,6 +62,12 @@
   </si>
   <si>
     <t xml:space="preserve">Generator beefed-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generator DCGAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100→512</t>
   </si>
   <si>
     <t xml:space="preserve">Generator UNET</t>
@@ -272,10 +278,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="C2:M95"/>
+  <dimension ref="C2:W95"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A53" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I85" activeCellId="0" sqref="I85"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L50" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q80" activeCellId="0" sqref="Q80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1276,6 +1282,17 @@
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
+      <c r="O63" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P63" s="2"/>
+      <c r="Q63" s="2"/>
+      <c r="R63" s="2"/>
+      <c r="S63" s="2"/>
+      <c r="T63" s="2"/>
+      <c r="U63" s="2"/>
+      <c r="V63" s="2"/>
+      <c r="W63" s="2"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D64" s="3" t="s">
@@ -1297,6 +1314,25 @@
       </c>
       <c r="K64" s="3"/>
       <c r="L64" s="3"/>
+      <c r="O64" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="P64" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q64" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="R64" s="3"/>
+      <c r="S64" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="T64" s="3"/>
+      <c r="U64" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="V64" s="3"/>
+      <c r="W64" s="3"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D65" s="2" t="n">
@@ -1320,6 +1356,31 @@
       <c r="L65" s="2" t="n">
         <f aca="false">(D65-1)*F65-2*J65+H65*(E65-1)+0+1</f>
         <v>3</v>
+      </c>
+      <c r="N65" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="O65" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="P65" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q65" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="R65" s="2"/>
+      <c r="S65" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T65" s="2"/>
+      <c r="U65" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V65" s="2"/>
+      <c r="W65" s="2" t="n">
+        <f aca="false">(O65-1)*Q65-2*U65+S65*(P65-1)+0+1</f>
+        <v>4</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1346,6 +1407,32 @@
         <f aca="false">(D66-1)*F66-2*J66+H66*(E66-1)+0+1</f>
         <v>7</v>
       </c>
+      <c r="N66" s="0" t="n">
+        <v>512</v>
+      </c>
+      <c r="O66" s="2" t="n">
+        <f aca="false">W65</f>
+        <v>4</v>
+      </c>
+      <c r="P66" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q66" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="R66" s="2"/>
+      <c r="S66" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T66" s="2"/>
+      <c r="U66" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="V66" s="2"/>
+      <c r="W66" s="2" t="n">
+        <f aca="false">(O66-1)*Q66-2*U66+S66*(P66-1)+0+1</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D67" s="2" t="n">
@@ -1371,6 +1458,32 @@
         <f aca="false">(D67-1)*F67-2*J67+H67*(E67-1)+0+1</f>
         <v>15</v>
       </c>
+      <c r="N67" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="O67" s="2" t="n">
+        <f aca="false">W66</f>
+        <v>8</v>
+      </c>
+      <c r="P67" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q67" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="R67" s="2"/>
+      <c r="S67" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T67" s="2"/>
+      <c r="U67" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="V67" s="2"/>
+      <c r="W67" s="2" t="n">
+        <f aca="false">(O67-1)*Q67-2*U67+S67*(P67-1)+0+1</f>
+        <v>16</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D68" s="2" t="n">
@@ -1396,6 +1509,32 @@
         <f aca="false">(D68-1)*F68-2*J68+H68*(E68-1)+0+1</f>
         <v>17</v>
       </c>
+      <c r="N68" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="O68" s="2" t="n">
+        <f aca="false">W67</f>
+        <v>16</v>
+      </c>
+      <c r="P68" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q68" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="R68" s="2"/>
+      <c r="S68" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T68" s="2"/>
+      <c r="U68" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="V68" s="2"/>
+      <c r="W68" s="2" t="n">
+        <f aca="false">(O68-1)*Q68-2*U68+S68*(P68-1)+0+1</f>
+        <v>32</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D69" s="2" t="n">
@@ -1421,6 +1560,32 @@
         <f aca="false">(D69-1)*F69-2*J69+H69*(E69-1)+0+1</f>
         <v>20</v>
       </c>
+      <c r="N69" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="O69" s="2" t="n">
+        <f aca="false">W68</f>
+        <v>32</v>
+      </c>
+      <c r="P69" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q69" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="R69" s="2"/>
+      <c r="S69" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T69" s="2"/>
+      <c r="U69" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="V69" s="2"/>
+      <c r="W69" s="2" t="n">
+        <f aca="false">(O69-1)*Q69-2*U69+S69*(P69-1)+0+1</f>
+        <v>64</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D70" s="2" t="n">
@@ -1446,6 +1611,32 @@
         <f aca="false">(D70-1)*F70-2*J70+H70*(E70-1)+0+1</f>
         <v>22</v>
       </c>
+      <c r="N70" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="O70" s="2" t="n">
+        <f aca="false">W69</f>
+        <v>64</v>
+      </c>
+      <c r="P70" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q70" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="R70" s="2"/>
+      <c r="S70" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T70" s="2"/>
+      <c r="U70" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="V70" s="2"/>
+      <c r="W70" s="2" t="n">
+        <f aca="false">(O70-1)*Q70-2*U70+S70*(P70-1)+0+1</f>
+        <v>128</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D71" s="2" t="n">
@@ -1471,6 +1662,32 @@
         <f aca="false">(D71-1)*F71-2*J71+H71*(E71-1)+0+1</f>
         <v>24</v>
       </c>
+      <c r="N71" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="O71" s="2" t="n">
+        <f aca="false">W70</f>
+        <v>128</v>
+      </c>
+      <c r="P71" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q71" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="R71" s="2"/>
+      <c r="S71" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T71" s="2"/>
+      <c r="U71" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="V71" s="2"/>
+      <c r="W71" s="2" t="n">
+        <f aca="false">(O71-1)*Q71-2*U71+S71*(P71-1)+0+1</f>
+        <v>256</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D72" s="2" t="n">
@@ -1571,10 +1788,196 @@
         <f aca="false">(D75-1)*F75-2*J75+H75*(E75-1)+0+1</f>
         <v>224</v>
       </c>
+      <c r="O75" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="P75" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q75" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="R75" s="3"/>
+      <c r="S75" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="T75" s="3"/>
+      <c r="U75" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="V75" s="3"/>
+      <c r="W75" s="3"/>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N76" s="0" t="n">
+        <v>512</v>
+      </c>
+      <c r="O76" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="P76" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q76" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="R76" s="2"/>
+      <c r="S76" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T76" s="2"/>
+      <c r="U76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V76" s="2"/>
+      <c r="W76" s="2" t="n">
+        <f aca="false">(O76-1)*Q76-2*U76+S76*(P76-1)+0+1</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N77" s="0" t="n">
+        <v>512</v>
+      </c>
+      <c r="O77" s="2" t="n">
+        <f aca="false">W76</f>
+        <v>4</v>
+      </c>
+      <c r="P77" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q77" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="R77" s="2"/>
+      <c r="S77" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T77" s="2"/>
+      <c r="U77" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="V77" s="2"/>
+      <c r="W77" s="2" t="n">
+        <f aca="false">(O77-1)*Q77-2*U77+S77*(P77-1)+0+1</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N78" s="0" t="n">
+        <v>512</v>
+      </c>
+      <c r="O78" s="2" t="n">
+        <f aca="false">W77</f>
+        <v>4</v>
+      </c>
+      <c r="P78" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q78" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="R78" s="2"/>
+      <c r="S78" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T78" s="2"/>
+      <c r="U78" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="V78" s="2"/>
+      <c r="W78" s="2" t="n">
+        <f aca="false">(O78-1)*Q78-2*U78+S78*(P78-1)+0+1</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N79" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="O79" s="2" t="n">
+        <f aca="false">W78</f>
+        <v>7</v>
+      </c>
+      <c r="P79" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q79" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="R79" s="2"/>
+      <c r="S79" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T79" s="2"/>
+      <c r="U79" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="V79" s="2"/>
+      <c r="W79" s="2" t="n">
+        <f aca="false">(O79-1)*Q79-2*U79+S79*(P79-1)+0+1</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N80" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="O80" s="2" t="n">
+        <f aca="false">W79</f>
+        <v>13</v>
+      </c>
+      <c r="P80" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q80" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="R80" s="2"/>
+      <c r="S80" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T80" s="2"/>
+      <c r="U80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V80" s="2"/>
+      <c r="W80" s="2" t="n">
+        <f aca="false">(O80-1)*Q80-2*U80+S80*(P80-1)+0+1</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N81" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="O81" s="2" t="n">
+        <f aca="false">W80</f>
+        <v>27</v>
+      </c>
+      <c r="P81" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q81" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="R81" s="2"/>
+      <c r="S81" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T81" s="2"/>
+      <c r="U81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V81" s="2"/>
+      <c r="W81" s="2" t="n">
+        <f aca="false">(O81-1)*Q81-2*U81+S81*(P81-1)+0+1</f>
+        <v>55</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D82" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
@@ -1584,33 +1987,85 @@
       <c r="J82" s="2"/>
       <c r="K82" s="2"/>
       <c r="L82" s="2"/>
+      <c r="N82" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="O82" s="2" t="n">
+        <f aca="false">W81</f>
+        <v>55</v>
+      </c>
+      <c r="P82" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q82" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="R82" s="2"/>
+      <c r="S82" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T82" s="2"/>
+      <c r="U82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V82" s="2"/>
+      <c r="W82" s="2" t="n">
+        <f aca="false">(O82-1)*Q82-2*U82+S82*(P82-1)+0+1</f>
+        <v>111</v>
+      </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D83" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H83" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I83" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="J83" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K83" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="L83" s="3"/>
+      <c r="N83" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="O83" s="2" t="n">
+        <f aca="false">W82</f>
+        <v>111</v>
+      </c>
+      <c r="P83" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q83" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="R83" s="2"/>
+      <c r="S83" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T83" s="2"/>
+      <c r="U83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V83" s="2"/>
+      <c r="W83" s="2" t="n">
+        <f aca="false">(O83-1)*Q83-2*U83+S83*(P83-1)+0+1</f>
+        <v>224</v>
+      </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D84" s="2" t="n">
@@ -1799,7 +2254,7 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C90" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D90" s="2" t="n">
         <f aca="false">L89</f>
@@ -1850,7 +2305,7 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C92" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D92" s="2" t="n">
         <f aca="false">L89</f>

</xml_diff>

<commit_message>
fix in unet lightning implementation
Signed-off-by: Augusto Luis Ballardini <augusto.ballardini@uah.es>
</commit_message>
<xml_diff>
--- a/GAN/GAN.layer.calculator.xlsx
+++ b/GAN/GAN.layer.calculator.xlsx
@@ -280,13 +280,13 @@
   </sheetPr>
   <dimension ref="C2:W95"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L50" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q80" activeCellId="0" sqref="Q80"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F72" activeCellId="0" sqref="F72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.12"/>
   </cols>
   <sheetData>
@@ -2264,7 +2264,7 @@
         <v>2</v>
       </c>
       <c r="F90" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G90" s="2"/>
       <c r="H90" s="2" t="n">
@@ -2281,7 +2281,7 @@
       </c>
       <c r="L90" s="2" t="n">
         <f aca="false">(D90*E90)-F90+2*G90-H90+2*I90-J90+2*K90+3</f>
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>